<commit_message>
Straight from Karbon v1
</commit_message>
<xml_diff>
--- a/excel_files/case_progress_risk.xlsx
+++ b/excel_files/case_progress_risk.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
   <si>
     <t>status</t>
   </si>
@@ -31,10 +31,10 @@
     <t>Clarification Required</t>
   </si>
   <si>
+    <t>Outreach Required</t>
+  </si>
+  <si>
     <t>In Progress</t>
-  </si>
-  <si>
-    <t>Outreach Required</t>
   </si>
   <si>
     <t>Low</t>
@@ -405,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -433,10 +433,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D2" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -447,10 +447,10 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -461,10 +461,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -475,10 +475,10 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>124</v>
       </c>
       <c r="D5" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -489,10 +489,10 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>142</v>
       </c>
       <c r="D6" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -503,10 +503,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>4</v>
+        <v>91</v>
       </c>
       <c r="D7" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -517,10 +517,10 @@
         <v>7</v>
       </c>
       <c r="C8">
-        <v>121</v>
+        <v>5</v>
       </c>
       <c r="D8" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -531,10 +531,10 @@
         <v>8</v>
       </c>
       <c r="C9">
-        <v>141</v>
+        <v>5</v>
       </c>
       <c r="D9" s="2">
-        <v>45499</v>
+        <v>45474</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -545,135 +545,9 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="D10" s="2">
-        <v>45499</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>30</v>
-      </c>
-      <c r="D11" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>6</v>
-      </c>
-      <c r="D13" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>5</v>
-      </c>
-      <c r="D14" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>5</v>
-      </c>
-      <c r="B15" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>4</v>
-      </c>
-      <c r="D16" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>124</v>
-      </c>
-      <c r="D17" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18">
-        <v>142</v>
-      </c>
-      <c r="D18" s="2">
-        <v>45474</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>91</v>
-      </c>
-      <c r="D19" s="2">
         <v>45474</v>
       </c>
     </row>

</xml_diff>